<commit_message>
Kleiner Fix an Ziele Tabell
</commit_message>
<xml_diff>
--- a/Ziele Tabelle.xlsx
+++ b/Ziele Tabelle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TOBI\Desktop\GourmetGuide\GourmetGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A00B8C0-E559-417F-AC93-250E91BA89EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322C3BED-7490-40BE-8CD9-DD00D7A8FA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Nr.</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Priorität</t>
   </si>
   <si>
-    <t>Feature</t>
-  </si>
-  <si>
     <t xml:space="preserve">Benutzerauthentifizierung </t>
   </si>
   <si>
@@ -88,6 +85,18 @@
   </si>
   <si>
     <t>Ein Benutzer soll, sofern angemeldet, Rezepte auf einer Sterneskala bewerten können</t>
+  </si>
+  <si>
+    <t>Leistung</t>
+  </si>
+  <si>
+    <t>Hauptziel</t>
+  </si>
+  <si>
+    <t>Funktionierendes Program</t>
+  </si>
+  <si>
+    <t>Es soll ein vollständig funkionierendes Program vorliegen</t>
   </si>
 </sst>
 </file>
@@ -148,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -163,6 +172,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -447,7 +459,7 @@
   <dimension ref="B2:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,16 +489,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -494,16 +506,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -511,16 +523,16 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -528,16 +540,16 @@
         <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -545,16 +557,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -562,24 +574,34 @@
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="F8" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ziele der Priorität nach geordnet
</commit_message>
<xml_diff>
--- a/Ziele Tabelle.xlsx
+++ b/Ziele Tabelle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TOBI\Desktop\GourmetGuide\GourmetGuide\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03HornT62\bitbucket\GourmetGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322C3BED-7490-40BE-8CD9-DD00D7A8FA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E420B567-8EB4-4B7F-80F6-75E77E5EB07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -157,24 +157,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,15 +455,17 @@
   <dimension ref="B2:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="6" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" customWidth="1"/>
+    <col min="4" max="4" width="23.08984375" customWidth="1"/>
+    <col min="5" max="6" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,127 +482,127 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3">
+    <row r="3" spans="2:6" ht="71.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5" t="s">
+    <row r="6" spans="2:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
+    <row r="7" spans="2:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5" t="s">
+    <row r="8" spans="2:6" ht="88" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3" t="s">
+    <row r="9" spans="2:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F9" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
-        <v>6</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:6" ht="50.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="2:6" ht="50.15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>